<commit_message>
added aspect sentiment columns to the training spreadsheet template
</commit_message>
<xml_diff>
--- a/datasets/template.xlsx
+++ b/datasets/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thrishnabhandari/Desktop/SummerProject2/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikita/Desktop/SummerProject2/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0DA757-65F5-1642-B2B3-96B3FA6652C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F3925D-4A2F-354B-80F5-D075DA92DCA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="1680" windowWidth="28040" windowHeight="16320" xr2:uid="{D2FFE28D-315C-7F45-8680-833170935627}"/>
+    <workbookView xWindow="1860" yWindow="6140" windowWidth="28040" windowHeight="16320" xr2:uid="{D2FFE28D-315C-7F45-8680-833170935627}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>sentence</t>
   </si>
@@ -81,6 +81,27 @@
   </si>
   <si>
     <t>character/world development</t>
+  </si>
+  <si>
+    <t>plot/story sentiment</t>
+  </si>
+  <si>
+    <t>acting sentiment</t>
+  </si>
+  <si>
+    <t>direction sentiment</t>
+  </si>
+  <si>
+    <t>cinemetography sentiment</t>
+  </si>
+  <si>
+    <t>editing sentiment</t>
+  </si>
+  <si>
+    <t>music sentiment</t>
+  </si>
+  <si>
+    <t>character/world development sentiment</t>
   </si>
 </sst>
 </file>
@@ -439,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A63DA1A-6BD4-1B4E-8D90-76818B839FCF}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,7 +477,7 @@
     <col min="12" max="12" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,85 +491,106 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="T1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="V1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="W1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>